<commit_message>
dodanie linków do Krotona
</commit_message>
<xml_diff>
--- a/plan/Rośliny.Zestawienie.xlsx
+++ b/plan/Rośliny.Zestawienie.xlsx
@@ -23,8 +23,420 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>user</author>
+  </authors>
+  <commentList>
+    <comment ref="B28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>koło skrzyni elektycznej</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+roślina 
+trochę inna niż proponowana</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+inny różowy niż Cheer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+inny fioletowy, nie Azurro
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+inny różwy, nie Elegant
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Kousa, ale biały
+jest też mnieszy za 32zł
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+trochę inna
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+czarny, ale BlackLace a nie Gerda
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+nie CrimsonPirate
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H67" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+rokitnica - też owoce jadalne</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H73" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+chiński</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H77" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+inny, Dwarf</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H97" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+inny</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H98" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+inny</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H107" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+inny</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H108" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+inna</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="324">
   <si>
     <t>Nr</t>
   </si>
@@ -793,9 +1205,6 @@
     <t>Średnia</t>
   </si>
   <si>
-    <t>Funkie są piękne :)</t>
-  </si>
-  <si>
     <t>Suma z Suma</t>
   </si>
   <si>
@@ -814,9 +1223,6 @@
     <t>Suma z Liczba (sztuki)</t>
   </si>
   <si>
-    <t>Opinie</t>
-  </si>
-  <si>
     <t>ok.</t>
   </si>
   <si>
@@ -826,19 +1232,10 @@
     <t>może być ich więcej</t>
   </si>
   <si>
-    <t>więcej funki</t>
-  </si>
-  <si>
     <t>miał być jeszcze rozmaryn</t>
   </si>
   <si>
     <t>inne byliny kwitnące</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +róża, piwonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - że niby czarny bez się rozplenia</t>
   </si>
   <si>
     <t xml:space="preserve">Hydrangea paniculata „Sundae Fraise Rensun” – Hortensja bukietowa, karłowa, różowa
@@ -1232,9 +1629,6 @@
     <t>160-180</t>
   </si>
   <si>
-    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.2629.oczar.posredni.pallida-hamamelis.x.intermedia.pallida.html</t>
-  </si>
-  <si>
     <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3373.fotergilla.amerykanska.-.fothergilla.major.html</t>
   </si>
   <si>
@@ -1389,13 +1783,112 @@
   </si>
   <si>
     <t>wysokosc rosliny</t>
+  </si>
+  <si>
+    <t>http://www.drzewa.com.pl/429-cyprysik-lawsona-columnaris.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.drzewa.com.pl/2966-zywotnik-zachodni-smaragd.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.drzewa.com.pl/2546-swierk-pospolity-cupressina.html?search_query=swierk+pospolity&amp;results=97</t>
+  </si>
+  <si>
+    <t>http://www.drzewa.com.pl/389-cis-posredni-hicksii.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.drzewa.com.pl/2046-sosna-czarna-pyramidata.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.mojsklepogrodniczy.pl/index.php?/Drzewa/Obni%BFki-cenowe/Cyprysik-Lawsona-na-%BFywop%B3ot-10-krzewow-%BFywop%B3otowych</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.mojsklepogrodniczy.pl/index.php?page=shop.browse&amp;option=com_virtuemart&amp;Itemid=27&amp;searchx=Y&amp;keyword=sosna+czarna&amp;search=Szukaj</t>
+  </si>
+  <si>
+    <t>15cm</t>
+  </si>
+  <si>
+    <t>Etap</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3768.trzmielina.oskrzydlona-.eunomynus.alatus.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.4524.rozanecznik.jakuszimanski.polaris.%E2%80%93.rhododendron.yakushimanum.%28y%29.polaris.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.4528.rozanecznik.jakuszimanski.%28y%29.caroline.allbrook%E2%80%93.rhododendron.yakushimanum.%28y%29.caroline.allbrook.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.4539.rozanecznik.wielkokwiatowy.germania.-.rhododendron.germania.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3222.deren.kousa.milky.way-cornus.cousa.milky.way.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.2776.kocimietka.faassena-nepeta.x.faassenii.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.1420.funkia.patriot.-.hosta.patriot.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3500.bez.czarny.black.lace-.sambucus.nigra.black.lace.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.4314.liliowiec.bestseller.-.hemerocallis.bestseller.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.2462.laurowisnia.otto.luyken.-prunus.laurocerasus.otto.luyken.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.2628.oczar.posredni.orange.beauty-hamamelis.x.intermedia.orange.beauty.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.2982.sadziec.dety.atropurpureum.-.eupatorium.atropurpureum.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3288.turzyca.oszimska.-.carex.oshimensis.evergold.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.2933.tawula.japonska.goldflame-.spiraea.japonica.goldflame.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3530.rokitnik.zwyczajny..hergo.-.hippophae.rhamnoides.l..hergo.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.4282.borowka.amerykanska.-.vaccinium.cor..bluegold.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.4547.borowka.amerykanska.pink.lemonade.rozowa.-.vaccinium.pink.lemonade.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3268.judaszowiec.chinski.avondale-cercis.chinensis.avondale.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3370.miskant.chinski.yakushima.dwarf.-.miscanthus.sinensis.yakushima.dwarf.html</t>
+  </si>
+  <si>
+    <t>http://www.ogrodkroton.pl/towar.4525.rozanecznik.jakuszimanski.morgenrot.%E2%80%93.rhododendron.yakushimanum.%28y%29.morgenrot.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.4526.rozanecznik.jakuszimanski.kalinka.%E2%80%93.rhododendron.yakushimanum.%28y%29.kalinka.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.1942.funkia.august.moon-.hosta.august.moon-.limonkowa.html</t>
+  </si>
+  <si>
+    <t>http://www.ogrodkroton.pl/towar.4626.rozchodnik.autumn.charm.-.sedum.autumn.charm.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3680.roza.gelbe.degmar.hastrup%C2%AE.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1528,6 +2021,73 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
@@ -1675,7 +2235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1876,41 +2436,29 @@
     <xf numFmtId="2" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="26" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2028,25 +2576,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
         <name val="Times New Roman"/>
@@ -2060,39 +2589,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2147,9 +2643,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2185,13 +2678,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
       </border>
     </dxf>
     <dxf>
@@ -2423,6 +2909,98 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2501,8 +3079,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>206775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>894938</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3977,7 +4555,7 @@
     <dataField name="Suma z Suma" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="3">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -3998,7 +4576,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="14">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -4019,7 +4597,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="2" selected="0">
@@ -4041,7 +4619,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="12">
       <pivotArea field="3" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2" selected="0">
@@ -4069,37 +4647,27 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:L118" totalsRowCount="1" headerRowDxfId="22" totalsRowDxfId="20" tableBorderDxfId="21">
   <autoFilter ref="A1:L117">
     <filterColumn colId="3"/>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="TAK"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="1"/>
-        <filter val="2"/>
-        <filter val="5"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
     <filterColumn colId="9"/>
     <filterColumn colId="10"/>
     <filterColumn colId="11"/>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="Nr" totalsRowLabel="Suma" totalsRowDxfId="19"/>
-    <tableColumn id="2" name="Nazwa" totalsRowDxfId="18"/>
-    <tableColumn id="3" name="Opis" totalsRowDxfId="17"/>
-    <tableColumn id="4" name="Typ" totalsRowDxfId="16"/>
-    <tableColumn id="5" name="Zimozielony?" totalsRowDxfId="15"/>
-    <tableColumn id="6" name="Strefa" totalsRowFunction="count" totalsRowDxfId="14"/>
-    <tableColumn id="7" name="Liczba (sztuki)" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="8" name="Średnia cena" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="9" name="Suma" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="1" name="Nr" totalsRowLabel="Suma" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Nazwa" totalsRowDxfId="10"/>
+    <tableColumn id="3" name="Opis" totalsRowDxfId="9"/>
+    <tableColumn id="4" name="Typ" totalsRowDxfId="8"/>
+    <tableColumn id="5" name="Zimozielony?" totalsRowDxfId="7"/>
+    <tableColumn id="6" name="Strefa" totalsRowFunction="count" totalsRowDxfId="6"/>
+    <tableColumn id="7" name="Liczba (sztuki)" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="5"/>
+    <tableColumn id="8" name="Średnia cena" totalsRowFunction="average" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="9" name="Suma" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="3">
       <calculatedColumnFormula>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Opinie" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="10" name="Sklep" totalsRowDxfId="5"/>
-    <tableColumn id="12" name="Wielkosc " totalsRowDxfId="4"/>
+    <tableColumn id="11" name="Etap" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="10" name="Sklep" totalsRowDxfId="1"/>
+    <tableColumn id="12" name="Wielkosc " totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4390,11 +4958,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P123"/>
+  <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:L74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4436,19 +5004,19 @@
         <v>95</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>172</v>
+        <v>299</v>
       </c>
       <c r="K1" s="59" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="L1" s="59" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="P1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="25.5" hidden="1">
+    <row r="2" spans="1:16" ht="22.5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4478,13 +5046,13 @@
         <v>100</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="25.5" hidden="1">
+    <row r="3" spans="1:16" ht="22.5">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4514,13 +5082,13 @@
         <v>70</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="25.5" hidden="1">
+    <row r="4" spans="1:16" ht="22.5">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -4550,13 +5118,13 @@
         <v>40</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26.25" hidden="1" customHeight="1">
+    <row r="5" spans="1:16" ht="26.25" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -4586,13 +5154,13 @@
         <v>200</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="38.25" hidden="1">
+    <row r="6" spans="1:16" ht="38.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -4622,13 +5190,13 @@
         <v>210</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:16" hidden="1">
+    <row r="7" spans="1:16">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -4658,18 +5226,18 @@
         <v>432</v>
       </c>
       <c r="J7" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="96" hidden="1">
+    <row r="8" spans="1:16" ht="96">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>96</v>
@@ -4700,7 +5268,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="38.25" hidden="1">
+    <row r="9" spans="1:16" ht="38.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -4730,13 +5298,13 @@
         <v>106.5</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="33.75" hidden="1">
+    <row r="10" spans="1:16" ht="33.75">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -4766,13 +5334,13 @@
         <v>120</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="45" hidden="1">
+    <row r="11" spans="1:16" ht="45">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -4800,10 +5368,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="45" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="45">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -4831,7 +5399,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="26.25" customHeight="1">
@@ -4864,7 +5432,7 @@
         <v>120</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="26.25" customHeight="1">
@@ -4872,7 +5440,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>4</v>
@@ -4895,7 +5463,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="26.25" customHeight="1">
@@ -4928,7 +5496,7 @@
         <v>110</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="26.25" customHeight="1">
@@ -4961,7 +5529,7 @@
         <v>35</v>
       </c>
       <c r="J16" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="24">
@@ -4992,7 +5560,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="22.5">
@@ -5025,13 +5593,13 @@
         <v>75</v>
       </c>
       <c r="J18" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K18" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="L18" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="33.75">
@@ -5062,10 +5630,10 @@
         <v>0</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="40.5" hidden="1" customHeight="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="40.5" customHeight="1">
       <c r="A20" s="5">
         <v>13</v>
       </c>
@@ -5093,15 +5661,15 @@
         <v>0</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="45" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="45">
       <c r="A21" s="5">
         <v>14</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>101</v>
@@ -5126,7 +5694,7 @@
         <v>35</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="36">
@@ -5157,7 +5725,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="24">
@@ -5190,13 +5758,13 @@
         <v>280</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K23" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="L23" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="24">
@@ -5219,23 +5787,23 @@
         <v>2</v>
       </c>
       <c r="G24" s="8">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H24" s="30">
         <v>9</v>
       </c>
       <c r="I24" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>243</v>
+        <v>279</v>
       </c>
       <c r="J24" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K24" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="L24" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="33.75">
@@ -5266,7 +5834,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="33.75">
@@ -5299,7 +5867,7 @@
         <v>40</v>
       </c>
       <c r="J26" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="25.5">
@@ -5330,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="25.5">
@@ -5356,14 +5924,17 @@
         <v>8</v>
       </c>
       <c r="H28" s="30">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I28" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="J28" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="K28" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="36">
@@ -5394,7 +5965,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="36">
@@ -5427,10 +5998,10 @@
         <v>120</v>
       </c>
       <c r="J30" s="37" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="56.25" hidden="1">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="56.25">
       <c r="A31" s="5">
         <v>19</v>
       </c>
@@ -5458,7 +6029,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="25.5">
@@ -5491,10 +6062,10 @@
         <v>40</v>
       </c>
       <c r="J32" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K32" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="45">
@@ -5525,7 +6096,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="33.75">
@@ -5556,7 +6127,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="69" customHeight="1">
@@ -5589,7 +6160,7 @@
         <v>120</v>
       </c>
       <c r="J35" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="67.5">
@@ -5597,10 +6168,10 @@
         <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>80</v>
@@ -5614,24 +6185,29 @@
       <c r="G36" s="8">
         <v>1</v>
       </c>
-      <c r="H36" s="30"/>
+      <c r="H36" s="30">
+        <v>32</v>
+      </c>
       <c r="I36" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="K36" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="56.25">
       <c r="A37" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>80</v>
@@ -5645,22 +6221,27 @@
       <c r="G37" s="8">
         <v>1</v>
       </c>
-      <c r="H37" s="30"/>
+      <c r="H37" s="30">
+        <v>28</v>
+      </c>
       <c r="I37" s="38">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J37" s="39"/>
+      <c r="K37" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="45">
       <c r="A38" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>80</v>
@@ -5674,22 +6255,27 @@
       <c r="G38" s="8">
         <v>1</v>
       </c>
-      <c r="H38" s="30"/>
+      <c r="H38" s="30">
+        <v>45</v>
+      </c>
       <c r="I38" s="38">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J38" s="39"/>
-    </row>
-    <row r="39" spans="1:12" ht="51" hidden="1">
+      <c r="K38" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="51">
       <c r="A39" s="5">
         <v>25</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>82</v>
@@ -5737,15 +6323,15 @@
         <v>90</v>
       </c>
       <c r="J40" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="144" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="144">
       <c r="A41" s="5">
         <v>27</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C41" s="41" t="s">
         <v>10</v>
@@ -5770,16 +6356,16 @@
         <v>39</v>
       </c>
       <c r="J41" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K41" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="L41" s="60" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" hidden="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="5">
         <v>28</v>
       </c>
@@ -5787,7 +6373,7 @@
         <v>43</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>80</v>
@@ -5807,10 +6393,10 @@
         <v>0</v>
       </c>
       <c r="J42" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="22.5" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="22.5">
       <c r="A43" s="5">
         <v>28</v>
       </c>
@@ -5838,10 +6424,10 @@
         <v>0</v>
       </c>
       <c r="J43" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="51" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="51">
       <c r="A44" s="5">
         <v>29</v>
       </c>
@@ -5869,7 +6455,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="33.75">
@@ -5902,10 +6488,10 @@
         <v>195</v>
       </c>
       <c r="J45" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="25.5" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="25.5">
       <c r="A46" s="5">
         <v>31</v>
       </c>
@@ -5928,14 +6514,17 @@
         <v>1</v>
       </c>
       <c r="H46" s="30">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="I46" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="J46" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="K46" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="24">
@@ -5968,10 +6557,10 @@
         <v>150</v>
       </c>
       <c r="J47" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="38.25" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="38.25">
       <c r="A48" s="5">
         <v>33</v>
       </c>
@@ -5994,17 +6583,20 @@
         <v>5</v>
       </c>
       <c r="H48" s="30">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="I48" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>20</v>
+        <v>37.5</v>
       </c>
       <c r="J48" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="33.75" hidden="1">
+        <v>171</v>
+      </c>
+      <c r="K48" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="33.75">
       <c r="A49" s="5">
         <v>34</v>
       </c>
@@ -6034,10 +6626,10 @@
         <v>84</v>
       </c>
       <c r="J49" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K49" t="s">
-        <v>165</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="38.25">
@@ -6070,10 +6662,10 @@
         <v>240</v>
       </c>
       <c r="J50" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="25.5" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="25.5">
       <c r="A51" s="5">
         <v>36</v>
       </c>
@@ -6096,17 +6688,17 @@
         <v>9</v>
       </c>
       <c r="H51" s="30">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="I51" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>1260</v>
+        <v>1080</v>
       </c>
       <c r="J51" s="37" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="33.75" hidden="1">
+    <row r="52" spans="1:12" ht="33.75">
       <c r="A52" s="5">
         <v>37</v>
       </c>
@@ -6129,17 +6721,20 @@
         <v>1</v>
       </c>
       <c r="H52" s="30">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I52" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J52" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="48" hidden="1">
+        <v>171</v>
+      </c>
+      <c r="K52" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="48">
       <c r="A53" s="5">
         <v>38</v>
       </c>
@@ -6162,14 +6757,17 @@
         <v>4</v>
       </c>
       <c r="H53" s="30">
-        <v>8</v>
+        <v>24.5</v>
       </c>
       <c r="I53" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="J53" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="K53" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="38.25">
@@ -6195,17 +6793,20 @@
         <v>6</v>
       </c>
       <c r="H54" s="30">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I54" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="J54" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="38.25" hidden="1">
+        <v>171</v>
+      </c>
+      <c r="K54" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="38.25">
       <c r="A55" s="5">
         <v>39</v>
       </c>
@@ -6233,7 +6834,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="24.75">
@@ -6256,20 +6857,20 @@
         <v>2</v>
       </c>
       <c r="G56" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H56" s="30">
         <v>150</v>
       </c>
       <c r="I56" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="J56" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="51" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="51">
       <c r="A57" s="5">
         <v>41</v>
       </c>
@@ -6292,20 +6893,20 @@
         <v>1</v>
       </c>
       <c r="H57" s="30">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="I57" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="J57" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K57" t="s">
-        <v>244</v>
+        <v>310</v>
       </c>
       <c r="L57" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -6338,10 +6939,10 @@
         <v>240</v>
       </c>
       <c r="J58" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="56.25" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="56.25">
       <c r="A59" s="5">
         <v>43</v>
       </c>
@@ -6364,17 +6965,20 @@
         <v>3</v>
       </c>
       <c r="H59" s="30">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="I59" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>30</v>
+        <v>40.5</v>
       </c>
       <c r="J59" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="22.5" hidden="1">
+        <v>171</v>
+      </c>
+      <c r="K59" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="22.5">
       <c r="A60" s="5">
         <v>44</v>
       </c>
@@ -6397,14 +7001,17 @@
         <v>5</v>
       </c>
       <c r="H60" s="30">
-        <v>7</v>
+        <v>9.5</v>
       </c>
       <c r="I60" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>35</v>
+        <v>47.5</v>
       </c>
       <c r="J60" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="K60" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="22.5">
@@ -6427,25 +7034,25 @@
         <v>2</v>
       </c>
       <c r="G61" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H61" s="30">
         <v>100</v>
       </c>
       <c r="I61" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="J61" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="24" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="24">
       <c r="A62" s="5">
         <v>46</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>10</v>
@@ -6470,16 +7077,16 @@
         <v>595</v>
       </c>
       <c r="J62" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K62" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="L62" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="45" hidden="1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="45">
       <c r="A63" s="5">
         <v>47</v>
       </c>
@@ -6509,10 +7116,10 @@
         <v>145</v>
       </c>
       <c r="J63" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K63" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="22.5">
@@ -6520,7 +7127,7 @@
         <v>48</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>13</v>
@@ -6543,10 +7150,10 @@
         <v>0</v>
       </c>
       <c r="J64" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="36" hidden="1" customHeight="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="36" customHeight="1">
       <c r="A65" s="5">
         <v>49</v>
       </c>
@@ -6576,13 +7183,13 @@
         <v>91</v>
       </c>
       <c r="J65" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K65" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="51" hidden="1">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="51">
       <c r="A66" s="5">
         <v>50</v>
       </c>
@@ -6605,17 +7212,20 @@
         <v>9</v>
       </c>
       <c r="H66" s="30">
-        <v>7</v>
+        <v>11.5</v>
       </c>
       <c r="I66" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>63</v>
+        <v>103.5</v>
       </c>
       <c r="J66" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="56.25" hidden="1">
+        <v>171</v>
+      </c>
+      <c r="K66" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="56.25">
       <c r="A67" s="12">
         <v>51</v>
       </c>
@@ -6638,15 +7248,18 @@
         <v>1</v>
       </c>
       <c r="H67" s="30">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="I67" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="J67" s="37"/>
-    </row>
-    <row r="68" spans="1:12" ht="56.25" hidden="1">
+      <c r="K67" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="56.25">
       <c r="A68" s="12">
         <v>52</v>
       </c>
@@ -6677,7 +7290,7 @@
       </c>
       <c r="J68" s="37"/>
     </row>
-    <row r="69" spans="1:12" ht="56.25" hidden="1">
+    <row r="69" spans="1:12" ht="56.25">
       <c r="A69" s="12">
         <v>53</v>
       </c>
@@ -6708,7 +7321,7 @@
       </c>
       <c r="J69" s="37"/>
     </row>
-    <row r="70" spans="1:12" ht="90" hidden="1">
+    <row r="70" spans="1:12" ht="90">
       <c r="A70" s="12">
         <v>54</v>
       </c>
@@ -6731,15 +7344,18 @@
         <v>1</v>
       </c>
       <c r="H70" s="30">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I70" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J70" s="37"/>
-    </row>
-    <row r="71" spans="1:12" ht="90" hidden="1">
+      <c r="K70" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="43.5" customHeight="1">
       <c r="A71" s="12">
         <v>55</v>
       </c>
@@ -6762,20 +7378,23 @@
         <v>2</v>
       </c>
       <c r="H71" s="30">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I71" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="J71" s="37"/>
-    </row>
-    <row r="72" spans="1:12" ht="84" hidden="1">
+      <c r="K71" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="84">
       <c r="A72" s="5">
         <v>56</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C72" s="16" t="s">
         <v>134</v>
@@ -6800,21 +7419,21 @@
         <v>75</v>
       </c>
       <c r="J72" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K72" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="L72" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="22.5" hidden="1">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="22.5">
       <c r="A73" s="5">
         <v>57</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>135</v>
@@ -6831,13 +7450,18 @@
       <c r="G73" s="8">
         <v>1</v>
       </c>
-      <c r="H73" s="30"/>
+      <c r="H73" s="30">
+        <v>85</v>
+      </c>
       <c r="I73" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="J73" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="K73" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="38.25">
@@ -6870,10 +7494,10 @@
         <v>75</v>
       </c>
       <c r="J74" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="33.75" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="33.75">
       <c r="A75" s="5">
         <v>59</v>
       </c>
@@ -6903,10 +7527,10 @@
         <v>48</v>
       </c>
       <c r="J75" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="22.5" hidden="1" customHeight="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="22.5" customHeight="1">
       <c r="A76" s="5">
         <v>60</v>
       </c>
@@ -6936,16 +7560,16 @@
         <v>180</v>
       </c>
       <c r="J76" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K76" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="L76" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="36" hidden="1">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="36">
       <c r="A77" s="5">
         <v>61</v>
       </c>
@@ -6975,10 +7599,13 @@
         <v>45</v>
       </c>
       <c r="J77" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="33.75" hidden="1">
+        <v>171</v>
+      </c>
+      <c r="K77" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="33.75">
       <c r="A78" s="5">
         <v>62</v>
       </c>
@@ -7008,13 +7635,13 @@
         <v>16</v>
       </c>
       <c r="J78" s="37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K78" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="45" hidden="1">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="45">
       <c r="A79" s="5">
         <v>63</v>
       </c>
@@ -7042,10 +7669,10 @@
         <v>0</v>
       </c>
       <c r="J79" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="33.75" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="33.75">
       <c r="A80" s="5">
         <v>64</v>
       </c>
@@ -7074,10 +7701,10 @@
       </c>
       <c r="J80" s="37"/>
       <c r="K80" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="25.5" hidden="1" customHeight="1">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="25.5" customHeight="1">
       <c r="A81" s="5">
         <v>65</v>
       </c>
@@ -7106,7 +7733,7 @@
       </c>
       <c r="J81" s="37"/>
     </row>
-    <row r="82" spans="1:10" ht="33.75" hidden="1">
+    <row r="82" spans="1:10" ht="33.75">
       <c r="A82" s="5">
         <v>66</v>
       </c>
@@ -7135,7 +7762,7 @@
       </c>
       <c r="J82" s="37"/>
     </row>
-    <row r="83" spans="1:10" ht="56.25" hidden="1">
+    <row r="83" spans="1:10" ht="56.25">
       <c r="A83" s="5">
         <v>67</v>
       </c>
@@ -7164,15 +7791,15 @@
       </c>
       <c r="J83" s="37"/>
     </row>
-    <row r="84" spans="1:10" ht="45" hidden="1">
+    <row r="84" spans="1:10" ht="45">
       <c r="A84" s="5">
         <v>68</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>88</v>
@@ -7192,10 +7819,10 @@
         <v>0</v>
       </c>
       <c r="J84" s="37" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="45" hidden="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="45">
       <c r="A85" s="5">
         <v>69</v>
       </c>
@@ -7223,10 +7850,10 @@
         <v>0</v>
       </c>
       <c r="J85" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="33.75" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="33.75">
       <c r="A86" s="5">
         <v>70</v>
       </c>
@@ -7256,10 +7883,10 @@
         <v>50</v>
       </c>
       <c r="J86" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="45" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="45">
       <c r="A87" s="5">
         <v>71</v>
       </c>
@@ -7287,10 +7914,10 @@
         <v>0</v>
       </c>
       <c r="J87" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="22.5" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="22.5">
       <c r="A88" s="5">
         <v>72</v>
       </c>
@@ -7318,10 +7945,10 @@
         <v>0</v>
       </c>
       <c r="J88" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="45" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="45">
       <c r="A89" s="5">
         <v>73</v>
       </c>
@@ -7349,10 +7976,10 @@
         <v>0</v>
       </c>
       <c r="J89" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="25.5" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="25.5">
       <c r="A90" s="5">
         <v>74</v>
       </c>
@@ -7380,10 +8007,10 @@
         <v>0</v>
       </c>
       <c r="J90" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="36" hidden="1" customHeight="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="36" customHeight="1">
       <c r="A91" s="5">
         <v>75</v>
       </c>
@@ -7411,10 +8038,10 @@
         <v>0</v>
       </c>
       <c r="J91" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="67.5" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="67.5">
       <c r="A92" s="5">
         <v>76</v>
       </c>
@@ -7442,10 +8069,10 @@
         <v>0</v>
       </c>
       <c r="J92" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="33.75" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="33.75">
       <c r="A93" s="5">
         <v>77</v>
       </c>
@@ -7473,10 +8100,10 @@
         <v>0</v>
       </c>
       <c r="J93" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="67.5" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="67.5">
       <c r="A94" s="5">
         <v>78</v>
       </c>
@@ -7506,10 +8133,10 @@
         <v>36</v>
       </c>
       <c r="J94" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="45" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="45">
       <c r="A95" s="5">
         <v>79</v>
       </c>
@@ -7539,15 +8166,15 @@
         <v>40</v>
       </c>
       <c r="J95" s="37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" hidden="1">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="15" thickBot="1">
       <c r="A96" s="5">
         <v>80</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>10</v>
@@ -7571,15 +8198,15 @@
       </c>
       <c r="J96" s="37"/>
     </row>
-    <row r="97" spans="1:12" ht="34.5" hidden="1" thickBot="1">
+    <row r="97" spans="1:12" ht="34.5" thickBot="1">
       <c r="A97" s="5">
         <v>81</v>
       </c>
       <c r="B97" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="52" t="s">
         <v>202</v>
-      </c>
-      <c r="C97" s="52" t="s">
-        <v>207</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>80</v>
@@ -7593,22 +8220,26 @@
       <c r="G97" s="8">
         <v>1</v>
       </c>
-      <c r="H97" s="30"/>
+      <c r="H97" s="30">
+        <v>28</v>
+      </c>
       <c r="I97" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
-      </c>
-      <c r="J97" s="37"/>
-    </row>
-    <row r="98" spans="1:12" ht="34.5" hidden="1" thickBot="1">
+        <v>28</v>
+      </c>
+      <c r="K97" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="34.5" thickBot="1">
       <c r="A98" s="5">
         <v>82</v>
       </c>
       <c r="B98" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C98" s="52" t="s">
         <v>203</v>
-      </c>
-      <c r="C98" s="52" t="s">
-        <v>208</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>80</v>
@@ -7622,22 +8253,26 @@
       <c r="G98" s="8">
         <v>1</v>
       </c>
-      <c r="H98" s="30"/>
+      <c r="H98" s="30">
+        <v>26</v>
+      </c>
       <c r="I98" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
-      </c>
-      <c r="J98" s="37"/>
-    </row>
-    <row r="99" spans="1:12" ht="57" hidden="1" thickBot="1">
+        <v>26</v>
+      </c>
+      <c r="K98" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="57" thickBot="1">
       <c r="A99" s="5">
         <v>83</v>
       </c>
       <c r="B99" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="C99" s="53" t="s">
         <v>204</v>
-      </c>
-      <c r="C99" s="53" t="s">
-        <v>209</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>80</v>
@@ -7660,21 +8295,21 @@
       </c>
       <c r="J99" s="37"/>
       <c r="K99" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="L99" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" ht="26.25" hidden="1" thickBot="1">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="26.25" thickBot="1">
       <c r="A100" s="5">
         <v>84</v>
       </c>
       <c r="B100" s="51" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C100" s="40" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>78</v>
@@ -7697,21 +8332,21 @@
       </c>
       <c r="J100" s="37"/>
       <c r="K100" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="L100" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" ht="57" hidden="1" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="57" thickBot="1">
       <c r="A101" s="5">
         <v>85</v>
       </c>
       <c r="B101" s="54" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C101" s="52" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>82</v>
@@ -7734,18 +8369,18 @@
       </c>
       <c r="J101" s="37"/>
       <c r="K101" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" ht="16.5" hidden="1" customHeight="1" thickBot="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A102" s="5">
         <v>86</v>
       </c>
       <c r="B102" s="50" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C102" s="40" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>80</v>
@@ -7759,22 +8394,24 @@
       <c r="G102" s="8">
         <v>6</v>
       </c>
-      <c r="H102" s="30"/>
+      <c r="H102" s="30">
+        <v>18.5</v>
+      </c>
       <c r="I102" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="J102" s="37"/>
     </row>
-    <row r="103" spans="1:12" ht="34.5" hidden="1" thickBot="1">
+    <row r="103" spans="1:12" ht="34.5" thickBot="1">
       <c r="A103" s="5">
         <v>87</v>
       </c>
       <c r="B103" s="51" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C103" s="52" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>82</v>
@@ -7795,15 +8432,15 @@
       </c>
       <c r="J103" s="37"/>
     </row>
-    <row r="104" spans="1:12" ht="45.75" hidden="1" thickBot="1">
+    <row r="104" spans="1:12" ht="45.75" thickBot="1">
       <c r="A104" s="5">
         <v>88</v>
       </c>
       <c r="B104" s="50" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C104" s="52" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>82</v>
@@ -7817,22 +8454,24 @@
       <c r="G104" s="8">
         <v>14</v>
       </c>
-      <c r="H104" s="30"/>
+      <c r="H104" s="30">
+        <v>17.5</v>
+      </c>
       <c r="I104" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="J104" s="37"/>
     </row>
-    <row r="105" spans="1:12" ht="57" hidden="1" thickBot="1">
+    <row r="105" spans="1:12" ht="57" thickBot="1">
       <c r="A105" s="5">
         <v>89</v>
       </c>
       <c r="B105" s="50" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C105" s="52" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>81</v>
@@ -7846,22 +8485,24 @@
       <c r="G105" s="8">
         <v>3</v>
       </c>
-      <c r="H105" s="30"/>
+      <c r="H105" s="30">
+        <v>10</v>
+      </c>
       <c r="I105" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J105" s="37"/>
     </row>
-    <row r="106" spans="1:12" ht="16.5" hidden="1" customHeight="1" thickBot="1">
+    <row r="106" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A106" s="5">
         <v>90</v>
       </c>
       <c r="B106" s="51" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C106" s="52" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>82</v>
@@ -7882,15 +8523,15 @@
       </c>
       <c r="J106" s="37"/>
     </row>
-    <row r="107" spans="1:12" ht="45.75" hidden="1" thickBot="1">
+    <row r="107" spans="1:12" ht="45.75" thickBot="1">
       <c r="A107" s="5">
         <v>91</v>
       </c>
       <c r="B107" s="50" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C107" s="52" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>82</v>
@@ -7904,22 +8545,27 @@
       <c r="G107" s="8">
         <v>3</v>
       </c>
-      <c r="H107" s="30"/>
+      <c r="H107" s="30">
+        <v>15</v>
+      </c>
       <c r="I107" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J107" s="37"/>
-    </row>
-    <row r="108" spans="1:12" ht="76.5" hidden="1">
+      <c r="K107" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="76.5">
       <c r="A108" s="5">
         <v>92</v>
       </c>
       <c r="B108" s="55" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C108" s="52" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>80</v>
@@ -7933,22 +8579,27 @@
       <c r="G108" s="8">
         <v>5</v>
       </c>
-      <c r="H108" s="30"/>
+      <c r="H108" s="30">
+        <v>28</v>
+      </c>
       <c r="I108" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="J108" s="37"/>
-    </row>
-    <row r="109" spans="1:12" ht="78.75" hidden="1">
+      <c r="K108" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="79.5" thickBot="1">
       <c r="A109" s="5">
         <v>93</v>
       </c>
       <c r="B109" s="56" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C109" s="52" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D109" s="8" t="s">
         <v>82</v>
@@ -7962,14 +8613,16 @@
       <c r="G109" s="8">
         <v>3</v>
       </c>
-      <c r="H109" s="30"/>
+      <c r="H109" s="30">
+        <v>65</v>
+      </c>
       <c r="I109" s="30">
         <f>Tabela1[[#This Row],[Liczba (sztuki)]]*Tabela1[[#This Row],[Średnia cena]]</f>
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="J109" s="37"/>
     </row>
-    <row r="110" spans="1:12" ht="45.75" hidden="1" thickBot="1">
+    <row r="110" spans="1:12" ht="45.75" thickBot="1">
       <c r="A110" s="5"/>
       <c r="B110" s="57" t="s">
         <v>32</v>
@@ -7996,7 +8649,7 @@
       </c>
       <c r="J110" s="37"/>
     </row>
-    <row r="111" spans="1:12" ht="45.75" hidden="1" thickBot="1">
+    <row r="111" spans="1:12" ht="45.75" thickBot="1">
       <c r="A111" s="5"/>
       <c r="B111" s="58" t="s">
         <v>60</v>
@@ -8025,7 +8678,7 @@
       </c>
       <c r="J111" s="37"/>
     </row>
-    <row r="112" spans="1:12" ht="45" hidden="1">
+    <row r="112" spans="1:12" ht="45">
       <c r="A112" s="5"/>
       <c r="B112" s="24" t="s">
         <v>61</v>
@@ -8052,7 +8705,7 @@
       </c>
       <c r="J112" s="37"/>
     </row>
-    <row r="113" spans="1:12" ht="45" hidden="1">
+    <row r="113" spans="1:12" ht="45">
       <c r="A113" s="5"/>
       <c r="B113" s="24" t="s">
         <v>62</v>
@@ -8081,7 +8734,7 @@
       </c>
       <c r="J113" s="37"/>
     </row>
-    <row r="114" spans="1:12" ht="33.75" hidden="1">
+    <row r="114" spans="1:12" ht="33.75">
       <c r="A114" s="5"/>
       <c r="B114" s="24" t="s">
         <v>63</v>
@@ -8108,7 +8761,7 @@
       </c>
       <c r="J114" s="37"/>
     </row>
-    <row r="115" spans="1:12" ht="42.75" hidden="1" customHeight="1">
+    <row r="115" spans="1:12" ht="42.75" customHeight="1">
       <c r="A115" s="5"/>
       <c r="B115" s="25" t="s">
         <v>64</v>
@@ -8137,7 +8790,7 @@
       </c>
       <c r="J115" s="37"/>
     </row>
-    <row r="116" spans="1:12" ht="33.75" hidden="1">
+    <row r="116" spans="1:12" ht="33.75">
       <c r="A116" s="5"/>
       <c r="B116" s="23" t="s">
         <v>33</v>
@@ -8166,7 +8819,7 @@
       </c>
       <c r="J116" s="37"/>
     </row>
-    <row r="117" spans="1:12" ht="33.75" hidden="1">
+    <row r="117" spans="1:12" ht="33.75">
       <c r="A117" s="28"/>
       <c r="B117" s="24" t="s">
         <v>65</v>
@@ -8195,7 +8848,7 @@
       </c>
       <c r="J117" s="37"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75">
+    <row r="118" spans="1:12" ht="24">
       <c r="A118" s="42" t="s">
         <v>95</v>
       </c>
@@ -8205,19 +8858,19 @@
       <c r="E118" s="45"/>
       <c r="F118" s="46">
         <f>SUBTOTAL(103,[Strefa])</f>
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="G118" s="46">
         <f>SUBTOTAL(109,[Liczba (sztuki)])</f>
-        <v>238</v>
+        <v>822</v>
       </c>
       <c r="H118" s="47">
         <f>SUBTOTAL(101,[Średnia cena])</f>
-        <v>30.2</v>
+        <v>33.540259740259742</v>
       </c>
       <c r="I118" s="46">
         <f>SUBTOTAL(109,[Suma])</f>
-        <v>3443</v>
+        <v>9395.5</v>
       </c>
       <c r="J118" s="46"/>
       <c r="K118" s="48"/>
@@ -8235,16 +8888,6 @@
       </c>
       <c r="I119" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12">
-      <c r="J122" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12">
-      <c r="J123" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -8256,8 +8899,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8297,27 +8941,27 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -8467,7 +9111,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" s="31">
         <v>52</v>
@@ -8495,10 +9139,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8508,24 +9152,24 @@
     <col min="7" max="7" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" t="s">
         <v>250</v>
       </c>
-      <c r="C1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D1" t="s">
-        <v>256</v>
-      </c>
       <c r="E1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
@@ -8533,17 +9177,17 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D2">
         <f>55*1.08</f>
         <v>59.400000000000006</v>
       </c>
       <c r="E2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="62" t="s">
         <v>43</v>
       </c>
@@ -8551,17 +9195,17 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D3">
         <f>55*1.08</f>
         <v>59.400000000000006</v>
       </c>
       <c r="E3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="62" t="s">
         <v>47</v>
       </c>
@@ -8569,17 +9213,17 @@
         <v>6</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D4">
         <f>15*1.08</f>
         <v>16.200000000000003</v>
       </c>
       <c r="E4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="62" t="s">
         <v>74</v>
       </c>
@@ -8587,55 +9231,55 @@
         <v>3</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D5">
         <f>15*1.08</f>
         <v>16.200000000000003</v>
       </c>
       <c r="E5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="22" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B6" s="8">
         <v>5</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D6">
         <f>15*1.08</f>
         <v>16.200000000000003</v>
       </c>
       <c r="E6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="C9" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E9" t="s">
+        <v>250</v>
+      </c>
+      <c r="F9" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="C9" t="s">
-        <v>255</v>
-      </c>
-      <c r="D9" t="s">
-        <v>250</v>
-      </c>
-      <c r="E9" t="s">
-        <v>256</v>
-      </c>
-      <c r="F9" t="s">
-        <v>257</v>
-      </c>
       <c r="G9" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="H9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="33" customHeight="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="33" customHeight="1">
       <c r="A10" s="65">
         <v>9</v>
       </c>
@@ -8643,63 +9287,60 @@
         <v>99</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="61">
-        <v>22</v>
-      </c>
-      <c r="E10" s="67">
-        <v>10</v>
-      </c>
-      <c r="F10" s="67">
-        <v>120</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="D10" s="61"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="68"/>
       <c r="H10" s="68"/>
     </row>
-    <row r="11" spans="1:8" ht="33" customHeight="1">
+    <row r="11" spans="1:9" ht="33" customHeight="1">
       <c r="A11" s="65"/>
       <c r="B11" s="64"/>
       <c r="C11" s="61"/>
       <c r="D11" s="61">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="67">
         <v>40</v>
       </c>
       <c r="F11" s="67">
-        <f t="shared" ref="F11:F36" si="0">E11*D11</f>
-        <v>880</v>
+        <f t="shared" ref="F11:F43" si="0">E11*D11</f>
+        <v>920</v>
       </c>
       <c r="G11" s="70" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H11" s="70" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="33" customHeight="1">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="33" customHeight="1">
       <c r="A12" s="65"/>
       <c r="B12" s="64"/>
       <c r="C12" s="61"/>
       <c r="D12" s="61">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="67">
         <v>18</v>
       </c>
       <c r="F12" s="67">
         <f t="shared" si="0"/>
-        <v>396</v>
+        <v>414</v>
       </c>
       <c r="G12" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="H12" s="70">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="33" customHeight="1">
+      <c r="I12">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="33" customHeight="1">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -8720,61 +9361,64 @@
         <v>310</v>
       </c>
       <c r="G13" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="H13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="33" customHeight="1">
-      <c r="A14" s="5">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="8">
-        <v>5</v>
-      </c>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="33" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E14" s="30">
         <v>25</v>
       </c>
       <c r="F14" s="30">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="G14" s="69" t="s">
-        <v>230</v>
-      </c>
-      <c r="H14" s="69" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="33" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="8"/>
+        <v>250</v>
+      </c>
+      <c r="G14" t="s">
+        <v>293</v>
+      </c>
+      <c r="H14" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="I14">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="33" customHeight="1">
+      <c r="A15" s="5">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="8">
+        <v>5</v>
+      </c>
       <c r="D15" s="8">
         <v>3</v>
       </c>
-      <c r="E15" s="30">
-        <v>10</v>
-      </c>
-      <c r="F15" s="30">
+      <c r="E15" s="74">
+        <v>25</v>
+      </c>
+      <c r="F15" s="74">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G15" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="H15" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="33" customHeight="1">
+        <v>75</v>
+      </c>
+      <c r="G15" s="73" t="s">
+        <v>225</v>
+      </c>
+      <c r="H15" s="69" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="33" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
@@ -8782,69 +9426,72 @@
         <v>3</v>
       </c>
       <c r="E16" s="30">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F16" s="30">
         <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="G16" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="H16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="33" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+      <c r="E17" s="30">
+        <v>26</v>
+      </c>
+      <c r="F17" s="30">
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="G16" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="H16" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="33" customHeight="1">
-      <c r="A17" s="65">
+      <c r="G17" s="69" t="s">
+        <v>275</v>
+      </c>
+      <c r="H17" t="s">
+        <v>276</v>
+      </c>
+      <c r="I17">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="33" customHeight="1">
+      <c r="A18" s="65">
         <v>15</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B18" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="61">
+      <c r="C18" s="61">
         <v>2.5</v>
       </c>
-      <c r="D17" s="61">
+      <c r="D18" s="75">
         <f>46-17</f>
         <v>29</v>
       </c>
-      <c r="E17" s="67">
+      <c r="E18" s="76">
         <v>9</v>
       </c>
-      <c r="F17" s="67">
+      <c r="F18" s="76">
         <f t="shared" si="0"/>
         <v>261</v>
       </c>
-      <c r="G17" t="s">
-        <v>230</v>
-      </c>
-      <c r="H17" s="70" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="33" customHeight="1">
-      <c r="A18" s="65"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61">
-        <v>29</v>
-      </c>
-      <c r="E18" s="67">
-        <v>10</v>
-      </c>
-      <c r="F18" s="67">
-        <f t="shared" si="0"/>
-        <v>290</v>
-      </c>
-      <c r="G18" t="s">
-        <v>285</v>
+      <c r="G18" s="77" t="s">
+        <v>225</v>
       </c>
       <c r="H18" s="70" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="33" customHeight="1">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="33" customHeight="1">
       <c r="A19" s="65"/>
       <c r="B19" s="63"/>
       <c r="C19" s="61"/>
@@ -8852,408 +9499,576 @@
         <v>29</v>
       </c>
       <c r="E19" s="67">
-        <v>3.75</v>
+        <v>10</v>
       </c>
       <c r="F19" s="67">
         <f t="shared" si="0"/>
-        <v>108.75</v>
+        <v>290</v>
       </c>
       <c r="G19" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="H19" s="70" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="33" customHeight="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="33" customHeight="1">
       <c r="A20" s="65"/>
       <c r="B20" s="63"/>
       <c r="C20" s="61"/>
-      <c r="D20" s="61">
-        <f>46-17</f>
+      <c r="D20" s="78">
         <v>29</v>
       </c>
-      <c r="E20" s="67">
-        <v>3.5</v>
-      </c>
-      <c r="F20" s="67">
+      <c r="E20" s="79">
+        <v>3.75</v>
+      </c>
+      <c r="F20" s="79">
         <f t="shared" si="0"/>
-        <v>101.5</v>
-      </c>
-      <c r="G20" t="s">
-        <v>259</v>
+        <v>108.75</v>
+      </c>
+      <c r="G20" s="80" t="s">
+        <v>255</v>
       </c>
       <c r="H20" s="70" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="33" customHeight="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="33" customHeight="1">
       <c r="A21" s="65"/>
       <c r="B21" s="63"/>
       <c r="C21" s="61"/>
       <c r="D21" s="61">
-        <v>17</v>
+        <f>46-17</f>
+        <v>29</v>
       </c>
       <c r="E21" s="67">
-        <v>35</v>
+        <v>3.5</v>
       </c>
       <c r="F21" s="67">
         <f t="shared" si="0"/>
-        <v>595</v>
+        <v>101.5</v>
       </c>
       <c r="G21" t="s">
-        <v>230</v>
-      </c>
-      <c r="H21" s="68" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="33" customHeight="1">
+        <v>253</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="33" customHeight="1">
       <c r="A22" s="65"/>
       <c r="B22" s="63"/>
       <c r="C22" s="61"/>
       <c r="D22" s="61">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E22" s="67">
-        <v>22</v>
+        <v>9.5</v>
       </c>
       <c r="F22" s="67">
-        <f t="shared" si="0"/>
-        <v>374</v>
+        <f>E22*D22</f>
+        <v>275.5</v>
       </c>
       <c r="G22" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="H22" s="70" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="33" customHeight="1">
+        <v>259</v>
+      </c>
+      <c r="I22">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="33" customHeight="1">
       <c r="A23" s="65"/>
       <c r="B23" s="63"/>
       <c r="C23" s="61"/>
-      <c r="D23" s="61">
+      <c r="D23" s="75">
         <v>17</v>
       </c>
-      <c r="E23" s="67">
+      <c r="E23" s="76">
+        <v>35</v>
+      </c>
+      <c r="F23" s="76">
+        <f t="shared" si="0"/>
+        <v>595</v>
+      </c>
+      <c r="G23" s="77" t="s">
+        <v>225</v>
+      </c>
+      <c r="H23" s="68" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="33" customHeight="1">
+      <c r="A24" s="65"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="78">
+        <v>17</v>
+      </c>
+      <c r="E24" s="79">
+        <v>22</v>
+      </c>
+      <c r="F24" s="79">
+        <f t="shared" si="0"/>
+        <v>374</v>
+      </c>
+      <c r="G24" s="80" t="s">
+        <v>266</v>
+      </c>
+      <c r="H24" s="70" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="33" customHeight="1">
+      <c r="A25" s="65"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61">
+        <v>17</v>
+      </c>
+      <c r="E25" s="67">
         <v>24</v>
       </c>
-      <c r="F23" s="67">
+      <c r="F25" s="67">
         <f t="shared" si="0"/>
         <v>408</v>
       </c>
-      <c r="G23" t="s">
-        <v>271</v>
-      </c>
-      <c r="H23" s="70" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="33" customHeight="1">
-      <c r="A24" s="65">
+      <c r="G25" t="s">
+        <v>265</v>
+      </c>
+      <c r="H25" s="70" t="s">
+        <v>258</v>
+      </c>
+      <c r="I25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="33" customHeight="1">
+      <c r="A26" s="65">
         <v>16</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B26" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="61">
+      <c r="C26" s="61">
         <v>2.5</v>
       </c>
-      <c r="D24" s="61">
+      <c r="D26" s="61">
         <v>5</v>
       </c>
-      <c r="E24" s="67">
+      <c r="E26" s="67">
         <v>14</v>
       </c>
-      <c r="F24" s="67">
+      <c r="F26" s="67">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="G24" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="H24" s="70" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A25" s="65">
+      <c r="G26" s="70" t="s">
+        <v>278</v>
+      </c>
+      <c r="H26" s="70" t="s">
+        <v>267</v>
+      </c>
+      <c r="I26">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="40.5" customHeight="1">
+      <c r="A27" s="65">
         <v>30</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B27" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="61">
+      <c r="C27" s="61">
         <v>2</v>
       </c>
-      <c r="D25" s="61">
+      <c r="D27" s="61">
         <v>13</v>
       </c>
-      <c r="E25" s="67">
+      <c r="E27" s="67">
         <v>11.5</v>
       </c>
-      <c r="F25" s="67">
+      <c r="F27" s="67">
         <f t="shared" si="0"/>
         <v>149.5</v>
       </c>
-      <c r="G25" s="70" t="s">
-        <v>266</v>
-      </c>
-      <c r="H25" s="70" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A26" s="65"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61">
+      <c r="G27" s="70" t="s">
+        <v>260</v>
+      </c>
+      <c r="H27" s="70" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="40.5" customHeight="1">
+      <c r="A28" s="65"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61">
         <v>13</v>
       </c>
-      <c r="E26" s="67">
+      <c r="E28" s="67">
         <v>14</v>
       </c>
-      <c r="F26" s="67">
+      <c r="F28" s="67">
         <f t="shared" si="0"/>
         <v>182</v>
       </c>
-      <c r="G26" s="70" t="s">
-        <v>275</v>
-      </c>
-      <c r="H26" s="70" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A27" s="65"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61">
+      <c r="G28" s="70" t="s">
+        <v>269</v>
+      </c>
+      <c r="H28" s="70" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="40.5" customHeight="1">
+      <c r="A29" s="65"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61">
         <v>13</v>
       </c>
-      <c r="E27" s="67">
+      <c r="E29" s="67">
         <v>29</v>
       </c>
-      <c r="F27" s="67">
+      <c r="F29" s="67">
         <f t="shared" si="0"/>
         <v>377</v>
       </c>
-      <c r="G27" t="s">
-        <v>276</v>
-      </c>
-      <c r="H27" s="70" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="33" customHeight="1">
-      <c r="A28" s="65">
+      <c r="G29" t="s">
+        <v>270</v>
+      </c>
+      <c r="H29" s="70" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="40.5" customHeight="1">
+      <c r="A30" s="65"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61">
+        <v>13</v>
+      </c>
+      <c r="E30" s="67">
+        <v>9</v>
+      </c>
+      <c r="F30" s="67">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="G30" t="s">
+        <v>291</v>
+      </c>
+      <c r="H30" s="70" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="40.5" customHeight="1">
+      <c r="A31" s="65"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61">
+        <v>13</v>
+      </c>
+      <c r="E31" s="67">
+        <v>4.7</v>
+      </c>
+      <c r="F31" s="67">
+        <f t="shared" si="0"/>
+        <v>61.1</v>
+      </c>
+      <c r="G31" s="70" t="s">
+        <v>296</v>
+      </c>
+      <c r="H31" s="70" t="s">
+        <v>286</v>
+      </c>
+      <c r="I31">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="33" customHeight="1">
+      <c r="A32" s="65">
         <v>35</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B32" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="61">
+      <c r="C32" s="61">
         <v>2</v>
       </c>
-      <c r="D28" s="61">
+      <c r="D32" s="61">
         <v>12</v>
       </c>
-      <c r="E28" s="67">
+      <c r="E32" s="67">
         <v>55</v>
       </c>
-      <c r="F28" s="67">
+      <c r="F32" s="67">
         <f t="shared" si="0"/>
         <v>660</v>
       </c>
-      <c r="G28" t="s">
-        <v>230</v>
-      </c>
-      <c r="H28" s="70" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="33" customHeight="1">
-      <c r="A29" s="65"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61">
+      <c r="G32" t="s">
+        <v>225</v>
+      </c>
+      <c r="H32" s="70" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="33" customHeight="1">
+      <c r="A33" s="65"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61">
         <v>12</v>
       </c>
-      <c r="E29" s="67">
-        <v>32</v>
-      </c>
-      <c r="F29" s="67">
-        <f t="shared" si="0"/>
-        <v>384</v>
-      </c>
-      <c r="G29" s="70" t="s">
-        <v>278</v>
-      </c>
-      <c r="H29" s="70" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="33" customHeight="1">
-      <c r="A30" s="65"/>
-      <c r="B30" s="62"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61">
+      <c r="E33" s="67">
         <v>12</v>
-      </c>
-      <c r="E30" s="67">
-        <v>14</v>
-      </c>
-      <c r="F30" s="67">
-        <f t="shared" si="0"/>
-        <v>168</v>
-      </c>
-      <c r="G30" s="70" t="s">
-        <v>288</v>
-      </c>
-      <c r="H30" s="70" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="33" customHeight="1">
-      <c r="A31" s="65"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61">
-        <v>12</v>
-      </c>
-      <c r="E31" s="67">
-        <v>11.5</v>
-      </c>
-      <c r="F31" s="67">
-        <f t="shared" si="0"/>
-        <v>138</v>
-      </c>
-      <c r="G31" t="s">
-        <v>267</v>
-      </c>
-      <c r="H31" s="70" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="33" customHeight="1">
-      <c r="A32" s="65"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61">
-        <v>12</v>
-      </c>
-      <c r="E32" s="67">
-        <v>1.4</v>
-      </c>
-      <c r="F32" s="67">
-        <f t="shared" si="0"/>
-        <v>16.799999999999997</v>
-      </c>
-      <c r="G32" t="s">
-        <v>260</v>
-      </c>
-      <c r="H32" s="70" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="33" customHeight="1">
-      <c r="A33" s="65">
-        <v>40</v>
-      </c>
-      <c r="B33" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="61">
-        <v>2</v>
-      </c>
-      <c r="D33" s="61">
-        <v>5</v>
-      </c>
-      <c r="E33" s="67">
-        <v>49</v>
       </c>
       <c r="F33" s="67">
         <f t="shared" si="0"/>
-        <v>245</v>
-      </c>
-      <c r="G33" s="70" t="s">
-        <v>289</v>
+        <v>144</v>
+      </c>
+      <c r="G33" t="s">
+        <v>294</v>
       </c>
       <c r="H33" s="70" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="33" customHeight="1">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="33" customHeight="1">
       <c r="A34" s="65"/>
       <c r="B34" s="62"/>
       <c r="C34" s="61"/>
       <c r="D34" s="61">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E34" s="67">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="F34" s="67">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>384</v>
       </c>
       <c r="G34" s="70" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H34" s="70" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="33" customHeight="1">
-      <c r="A35" s="65">
-        <v>45</v>
-      </c>
-      <c r="B35" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="61">
-        <v>2</v>
-      </c>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="33" customHeight="1">
+      <c r="A35" s="65"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="61">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E35" s="67">
-        <v>48.3</v>
+        <v>14</v>
       </c>
       <c r="F35" s="67">
         <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="G35" s="70" t="s">
+        <v>282</v>
+      </c>
+      <c r="H35" s="70" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="33" customHeight="1">
+      <c r="A36" s="65"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61">
+        <v>12</v>
+      </c>
+      <c r="E36" s="67">
+        <v>11.5</v>
+      </c>
+      <c r="F36" s="67">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="G36" t="s">
+        <v>261</v>
+      </c>
+      <c r="H36" s="70" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="33" customHeight="1">
+      <c r="A37" s="65"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78">
+        <v>12</v>
+      </c>
+      <c r="E37" s="79">
+        <v>1.4</v>
+      </c>
+      <c r="F37" s="79">
+        <f t="shared" si="0"/>
+        <v>16.799999999999997</v>
+      </c>
+      <c r="G37" s="80" t="s">
+        <v>254</v>
+      </c>
+      <c r="H37" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="I37">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="33" customHeight="1">
+      <c r="A38" s="65">
+        <v>40</v>
+      </c>
+      <c r="B38" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="61">
+        <v>2</v>
+      </c>
+      <c r="D38" s="61">
+        <v>5</v>
+      </c>
+      <c r="E38" s="67">
+        <v>49</v>
+      </c>
+      <c r="F38" s="67">
+        <f t="shared" si="0"/>
+        <v>245</v>
+      </c>
+      <c r="G38" s="70" t="s">
+        <v>283</v>
+      </c>
+      <c r="H38" s="70" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="33" customHeight="1">
+      <c r="A39" s="65"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61">
+        <v>5</v>
+      </c>
+      <c r="E39" s="67">
+        <v>25</v>
+      </c>
+      <c r="F39" s="67">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="G39" s="70" t="s">
+        <v>295</v>
+      </c>
+      <c r="H39" s="70" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="33" customHeight="1">
+      <c r="A40" s="65"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61">
+        <v>5</v>
+      </c>
+      <c r="E40" s="67">
+        <v>15</v>
+      </c>
+      <c r="F40" s="67">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G40" s="70" t="s">
+        <v>268</v>
+      </c>
+      <c r="H40" s="70" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="33" customHeight="1">
+      <c r="A41" s="65"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61">
+        <v>5</v>
+      </c>
+      <c r="E41" s="67">
+        <v>27</v>
+      </c>
+      <c r="F41" s="67">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="G41" s="70" t="s">
+        <v>297</v>
+      </c>
+      <c r="H41" s="70" t="s">
+        <v>298</v>
+      </c>
+      <c r="I41">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="33" customHeight="1">
+      <c r="A42" s="65">
+        <v>45</v>
+      </c>
+      <c r="B42" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="61">
+        <v>2</v>
+      </c>
+      <c r="D42" s="61">
+        <v>3</v>
+      </c>
+      <c r="E42" s="67">
+        <v>48.3</v>
+      </c>
+      <c r="F42" s="67">
+        <f t="shared" si="0"/>
         <v>144.89999999999998</v>
       </c>
-      <c r="G35" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H35" s="70" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="33" customHeight="1">
-      <c r="D36" s="71">
+      <c r="G42" s="70" t="s">
+        <v>277</v>
+      </c>
+      <c r="H42" s="70" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="33" customHeight="1">
+      <c r="D43" s="71">
         <v>3</v>
       </c>
-      <c r="E36" s="72">
+      <c r="E43" s="72">
         <v>26</v>
       </c>
-      <c r="F36" s="72">
+      <c r="F43" s="72">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="G36" s="70" t="s">
-        <v>293</v>
-      </c>
-      <c r="H36" s="70" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="33" customHeight="1"/>
-    <row r="38" spans="1:8" ht="33" customHeight="1"/>
-    <row r="39" spans="1:8" ht="33" customHeight="1"/>
-    <row r="40" spans="1:8" ht="33" customHeight="1"/>
+      <c r="G43" s="70" t="s">
+        <v>287</v>
+      </c>
+      <c r="H43" s="70" t="s">
+        <v>274</v>
+      </c>
+      <c r="I43">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="33" customHeight="1"/>
+    <row r="45" spans="1:9" ht="33" customHeight="1"/>
+    <row r="46" spans="1:9" ht="33" customHeight="1"/>
+    <row r="47" spans="1:9" ht="33" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wybór sklepów na iglaki
</commit_message>
<xml_diff>
--- a/plan/Rośliny.Zestawienie.xlsx
+++ b/plan/Rośliny.Zestawienie.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20400" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20400" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Zestawienie" sheetId="1" r:id="rId1"/>
     <sheet name="Statystyki" sheetId="2" r:id="rId2"/>
     <sheet name="Iglaki" sheetId="3" r:id="rId3"/>
-    <sheet name="Arkusz2" sheetId="4" r:id="rId4"/>
+    <sheet name="sklepy" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Zestawienie!$A$1:$I$117</definedName>
@@ -436,7 +436,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="432">
   <si>
     <t>Nr</t>
   </si>
@@ -1883,12 +1883,360 @@
   <si>
     <t xml:space="preserve"> http://www.ogrodkroton.pl/towar.3680.roza.gelbe.degmar.hastrup%C2%AE.html</t>
   </si>
+  <si>
+    <t>bartak 14zł</t>
+  </si>
+  <si>
+    <t>bartak 15zł</t>
+  </si>
+  <si>
+    <t>Szukane po Opineo.pl:</t>
+  </si>
+  <si>
+    <t>http://www.opineo.pl/opinie/euroogrod-com-pl</t>
+  </si>
+  <si>
+    <t>http://www.opineo.pl/opinie/iglaki24-pl</t>
+  </si>
+  <si>
+    <t>http://www.opineo.pl/opinie/iglaco-com</t>
+  </si>
+  <si>
+    <t>http://www.opineo.pl/opinie/sadowniczy-pl</t>
+  </si>
+  <si>
+    <t>http://www.opineo.pl/opinie/ogrodkroton-pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szukane po top sprzedaży „Tuja” na allegro: </t>
+  </si>
+  <si>
+    <t>www_e-iglaki_p (e-iglaki.pl)</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=19723221</t>
+  </si>
+  <si>
+    <t>sadzonki.org</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=40421692</t>
+  </si>
+  <si>
+    <t>e-market_24h (http://zielony-zywoplot.pl)</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=9600079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szukane po top  sprzedaży „Miskant” na allegro: </t>
+  </si>
+  <si>
+    <t>Gladi20 (http://www.gardenpark.com.pl)</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=386018</t>
+  </si>
+  <si>
+    <t>akex-Albamar</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=7792153</t>
+  </si>
+  <si>
+    <t>asiagaw</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=2192767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szukane po top10  sprzedaży http://allegro.pl/rosliny-drzewa-i-krzewy-iglaste-99745 na allegro: </t>
+  </si>
+  <si>
+    <t>gladi20</t>
+  </si>
+  <si>
+    <t>flora-top1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akex-Albamar </t>
+  </si>
+  <si>
+    <t>Mayla_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szukane po top10  sprzedaży http://allegro.pl/rosliny-trawy-99817 na allegro: </t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=40021923</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=27500783</t>
+  </si>
+  <si>
+    <t>miododajne</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=16855451</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szukane po top20  sprzedaży http://allegro.pl/rosliny-drzewa-i-krzewy-lisciaste-99754 na allegro: </t>
+  </si>
+  <si>
+    <t>e-market_24h</t>
+  </si>
+  <si>
+    <t>podkarpackie sady</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=24173211</t>
+  </si>
+  <si>
+    <t>Szutniczek</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=3673023</t>
+  </si>
+  <si>
+    <t>smilingface</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=5451084</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">farus22 (sadzonki po 2PLN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=29276533</t>
+  </si>
+  <si>
+    <t>Ogrod-marzen</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/show_user.php?uid=17390038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szukane po top15  sprzedaży http://allegro.pl/rosliny-byliny-ozdobne-99806  na allegro: </t>
+  </si>
+  <si>
+    <t>Lista docelowa</t>
+  </si>
+  <si>
+    <t>Euroogrod</t>
+  </si>
+  <si>
+    <t>Lista pośrednia</t>
+  </si>
+  <si>
+    <t>nie tylko rośliny</t>
+  </si>
+  <si>
+    <t>iglaki, drzewa i krzewy  llisc, azalie'</t>
+  </si>
+  <si>
+    <t>100% opineo</t>
+  </si>
+  <si>
+    <t>Iglaki24</t>
+  </si>
+  <si>
+    <t>mało sprzedali, nawet na allegro ma 96,5%</t>
+  </si>
+  <si>
+    <t>duzo roslin</t>
+  </si>
+  <si>
+    <t>Iglaco com</t>
+  </si>
+  <si>
+    <t>troche mało roślin</t>
+  </si>
+  <si>
+    <t>99 opineo,  allegro 99,3%, duzo sprzedali</t>
+  </si>
+  <si>
+    <t>92 opineo(1000 opinii), chyba ich nie ma na allegro</t>
+  </si>
+  <si>
+    <t>niewiele, głownie owocowe</t>
+  </si>
+  <si>
+    <t>Sadowniczy</t>
+  </si>
+  <si>
+    <t>Kroton</t>
+  </si>
+  <si>
+    <t>słabe opinie</t>
+  </si>
+  <si>
+    <t>bardzo duzy wybór</t>
+  </si>
+  <si>
+    <t>zielony - ok.</t>
+  </si>
+  <si>
+    <t>granatowy - do zastaniwenia</t>
+  </si>
+  <si>
+    <t>czerwony - odrzucony</t>
+  </si>
+  <si>
+    <t>tylko jeśli wybór i odbiór osobisty</t>
+  </si>
+  <si>
+    <t>e-iglaki.pl</t>
+  </si>
+  <si>
+    <t>allegro mała sprzedaz 4000, 96,4%</t>
+  </si>
+  <si>
+    <t>drzewa, krzewy , głownie iglaki</t>
+  </si>
+  <si>
+    <t>sadzonki,org</t>
+  </si>
+  <si>
+    <t>allegro mały spzrdaz 900, 97%</t>
+  </si>
+  <si>
+    <t>glad20</t>
+  </si>
+  <si>
+    <t>sallegro 85000, 99,4%</t>
+  </si>
+  <si>
+    <t>mały wybór</t>
+  </si>
+  <si>
+    <t>market24h</t>
+  </si>
+  <si>
+    <t>3000 allegro, 98,5%</t>
+  </si>
+  <si>
+    <t>ma rosliny zywoplowtowe</t>
+  </si>
+  <si>
+    <t>akekx albamar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130tys allegro, </t>
+  </si>
+  <si>
+    <t>nie ma iglaków, duzo bylin, trawy</t>
+  </si>
+  <si>
+    <t>32000, 98,5% allegro</t>
+  </si>
+  <si>
+    <t>nie ma igaków, głownie byliny, trawy</t>
+  </si>
+  <si>
+    <t>floratop1</t>
+  </si>
+  <si>
+    <t>1600 allegro, 99,8%</t>
+  </si>
+  <si>
+    <t>za mały wybór</t>
+  </si>
+  <si>
+    <t>mayla_pl</t>
+  </si>
+  <si>
+    <t>4600 allegro, 98,3%</t>
+  </si>
+  <si>
+    <t>głownie byliny trawy, nie kupują tui</t>
+  </si>
+  <si>
+    <t>47000, 100% allegro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duzo drzew lisciastych, </t>
+  </si>
+  <si>
+    <t>podkarpackiesady</t>
+  </si>
+  <si>
+    <t>allegro 47000 dobrze99,7</t>
+  </si>
+  <si>
+    <t>szutniczek</t>
+  </si>
+  <si>
+    <t>głównie lisciaste</t>
+  </si>
+  <si>
+    <t>24000, 98,8%</t>
+  </si>
+  <si>
+    <t>50000, 99,6%</t>
+  </si>
+  <si>
+    <t>nie ma iglakow, lisciaste i byliny, troche funkii</t>
+  </si>
+  <si>
+    <t>farus22</t>
+  </si>
+  <si>
+    <t>dlownie lisciaste, tanie pierdki</t>
+  </si>
+  <si>
+    <t>ogrod-marzen</t>
+  </si>
+  <si>
+    <t>65000, 99%</t>
+  </si>
+  <si>
+    <t>ma iglaste, lisciaste</t>
+  </si>
+  <si>
+    <t>iglak1</t>
+  </si>
+  <si>
+    <t>iglak2</t>
+  </si>
+  <si>
+    <t>sklep1</t>
+  </si>
+  <si>
+    <t>sklep2</t>
+  </si>
+  <si>
+    <t>cena, wysokosc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="28">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;zł&quot;;[Red]\-#,##0\ &quot;zł&quot;"/>
+  </numFmts>
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2090,8 +2438,64 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2120,6 +2524,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2232,10 +2642,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2454,8 +2868,38 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
@@ -3079,8 +3523,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>206775</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>894938</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>430697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4646,9 +5090,21 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:L118" totalsRowCount="1" headerRowDxfId="22" totalsRowDxfId="20" tableBorderDxfId="21">
   <autoFilter ref="A1:L117">
-    <filterColumn colId="3"/>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Drzewo"/>
+        <filter val="Drzewo małe"/>
+        <filter val="Krzew"/>
+        <filter val="Krzew mały"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4"/>
-    <filterColumn colId="5"/>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="9"/>
     <filterColumn colId="10"/>
     <filterColumn colId="11"/>
@@ -4961,8 +5417,8 @@
   <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5016,7 +5472,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="22.5">
+    <row r="2" spans="1:16" ht="25.5" hidden="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5052,7 +5508,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="22.5">
+    <row r="3" spans="1:16" ht="25.5" hidden="1">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -5088,7 +5544,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="22.5">
+    <row r="4" spans="1:16" ht="25.5" hidden="1">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -5124,7 +5580,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26.25" customHeight="1">
+    <row r="5" spans="1:16" ht="26.25" hidden="1" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -5160,7 +5616,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="38.25">
+    <row r="6" spans="1:16" ht="38.25" hidden="1">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -5196,7 +5652,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" hidden="1">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -5232,7 +5688,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="96">
+    <row r="8" spans="1:16" ht="96" hidden="1">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -5268,7 +5724,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="38.25">
+    <row r="9" spans="1:16" ht="38.25" hidden="1">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -5304,7 +5760,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="33.75">
+    <row r="10" spans="1:16" ht="33.75" hidden="1">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -5340,7 +5796,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="45">
+    <row r="11" spans="1:16" ht="45" hidden="1">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -5371,7 +5827,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="45">
+    <row r="12" spans="1:16" ht="45" hidden="1">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -5435,7 +5891,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="26.25" customHeight="1">
+    <row r="14" spans="1:16" ht="26.25" hidden="1" customHeight="1">
       <c r="A14" s="5">
         <v>9</v>
       </c>
@@ -5532,7 +5988,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="24">
+    <row r="17" spans="1:12" ht="24" hidden="1">
       <c r="A17" s="5">
         <v>10</v>
       </c>
@@ -5563,7 +6019,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="22.5">
+    <row r="18" spans="1:12" ht="22.5" hidden="1">
       <c r="A18" s="5">
         <v>11</v>
       </c>
@@ -5602,7 +6058,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="33.75">
+    <row r="19" spans="1:12" ht="33.75" hidden="1">
       <c r="A19" s="5">
         <v>12</v>
       </c>
@@ -5633,7 +6089,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="40.5" customHeight="1">
+    <row r="20" spans="1:12" ht="40.5" hidden="1" customHeight="1">
       <c r="A20" s="5">
         <v>13</v>
       </c>
@@ -5664,7 +6120,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="45">
+    <row r="21" spans="1:12" ht="45" hidden="1">
       <c r="A21" s="5">
         <v>14</v>
       </c>
@@ -5697,7 +6153,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="36">
+    <row r="22" spans="1:12" ht="36" hidden="1">
       <c r="A22" s="5" t="s">
         <v>109</v>
       </c>
@@ -5728,7 +6184,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="24">
+    <row r="23" spans="1:12" ht="24" hidden="1">
       <c r="A23" s="5">
         <v>15</v>
       </c>
@@ -5806,7 +6262,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="33.75">
+    <row r="25" spans="1:12" ht="33.75" hidden="1">
       <c r="A25" s="5">
         <v>16</v>
       </c>
@@ -5870,7 +6326,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="25.5">
+    <row r="27" spans="1:12" ht="25.5" hidden="1">
       <c r="A27" s="5">
         <v>17</v>
       </c>
@@ -5937,7 +6393,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="36">
+    <row r="29" spans="1:12" ht="36" hidden="1">
       <c r="A29" s="5">
         <v>18</v>
       </c>
@@ -6001,7 +6457,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="56.25">
+    <row r="31" spans="1:12" ht="56.25" hidden="1">
       <c r="A31" s="5">
         <v>19</v>
       </c>
@@ -6032,7 +6488,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="25.5">
+    <row r="32" spans="1:12" ht="25.5" hidden="1">
       <c r="A32" s="5">
         <v>20</v>
       </c>
@@ -6068,7 +6524,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="45">
+    <row r="33" spans="1:12" ht="45" hidden="1">
       <c r="A33" s="5">
         <v>21</v>
       </c>
@@ -6099,7 +6555,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="33.75">
+    <row r="34" spans="1:12" ht="33.75" hidden="1">
       <c r="A34" s="5">
         <v>22</v>
       </c>
@@ -6267,7 +6723,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="51">
+    <row r="39" spans="1:12" ht="51" hidden="1">
       <c r="A39" s="5">
         <v>25</v>
       </c>
@@ -6365,7 +6821,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" hidden="1">
       <c r="A42" s="5">
         <v>28</v>
       </c>
@@ -6396,7 +6852,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="22.5">
+    <row r="43" spans="1:12" ht="22.5" hidden="1">
       <c r="A43" s="5">
         <v>28</v>
       </c>
@@ -6427,7 +6883,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="51">
+    <row r="44" spans="1:12" ht="51" hidden="1">
       <c r="A44" s="5">
         <v>29</v>
       </c>
@@ -6560,7 +7016,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="38.25">
+    <row r="48" spans="1:12" ht="38.25" hidden="1">
       <c r="A48" s="5">
         <v>33</v>
       </c>
@@ -6596,7 +7052,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="33.75">
+    <row r="49" spans="1:12" ht="33.75" hidden="1">
       <c r="A49" s="5">
         <v>34</v>
       </c>
@@ -6734,7 +7190,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="48">
+    <row r="53" spans="1:12" ht="48" hidden="1">
       <c r="A53" s="5">
         <v>38</v>
       </c>
@@ -6806,7 +7262,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="38.25">
+    <row r="55" spans="1:12" ht="38.25" hidden="1">
       <c r="A55" s="5">
         <v>39</v>
       </c>
@@ -6942,7 +7398,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="56.25">
+    <row r="59" spans="1:12" ht="56.25" hidden="1">
       <c r="A59" s="5">
         <v>43</v>
       </c>
@@ -6978,7 +7434,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="22.5">
+    <row r="60" spans="1:12" ht="22.5" hidden="1">
       <c r="A60" s="5">
         <v>44</v>
       </c>
@@ -7153,7 +7609,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="36" customHeight="1">
+    <row r="65" spans="1:12" ht="36" hidden="1" customHeight="1">
       <c r="A65" s="5">
         <v>49</v>
       </c>
@@ -7497,7 +7953,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="33.75">
+    <row r="75" spans="1:12" ht="33.75" hidden="1">
       <c r="A75" s="5">
         <v>59</v>
       </c>
@@ -7530,7 +7986,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="22.5" customHeight="1">
+    <row r="76" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
       <c r="A76" s="5">
         <v>60</v>
       </c>
@@ -7569,7 +8025,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="36">
+    <row r="77" spans="1:12" ht="36.75" hidden="1" thickBot="1">
       <c r="A77" s="5">
         <v>61</v>
       </c>
@@ -7605,7 +8061,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="33.75">
+    <row r="78" spans="1:12" ht="34.5" hidden="1" thickBot="1">
       <c r="A78" s="5">
         <v>62</v>
       </c>
@@ -7641,7 +8097,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="45">
+    <row r="79" spans="1:12" ht="45.75" hidden="1" thickBot="1">
       <c r="A79" s="5">
         <v>63</v>
       </c>
@@ -7672,7 +8128,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="33.75">
+    <row r="80" spans="1:12" ht="34.5" hidden="1" thickBot="1">
       <c r="A80" s="5">
         <v>64</v>
       </c>
@@ -7704,7 +8160,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="25.5" customHeight="1">
+    <row r="81" spans="1:10" ht="25.5" hidden="1" customHeight="1">
       <c r="A81" s="5">
         <v>65</v>
       </c>
@@ -7733,7 +8189,7 @@
       </c>
       <c r="J81" s="37"/>
     </row>
-    <row r="82" spans="1:10" ht="33.75">
+    <row r="82" spans="1:10" ht="34.5" hidden="1" thickBot="1">
       <c r="A82" s="5">
         <v>66</v>
       </c>
@@ -7762,7 +8218,7 @@
       </c>
       <c r="J82" s="37"/>
     </row>
-    <row r="83" spans="1:10" ht="56.25">
+    <row r="83" spans="1:10" ht="57" hidden="1" thickBot="1">
       <c r="A83" s="5">
         <v>67</v>
       </c>
@@ -7791,7 +8247,7 @@
       </c>
       <c r="J83" s="37"/>
     </row>
-    <row r="84" spans="1:10" ht="45">
+    <row r="84" spans="1:10" ht="45.75" hidden="1" thickBot="1">
       <c r="A84" s="5">
         <v>68</v>
       </c>
@@ -7822,7 +8278,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="45">
+    <row r="85" spans="1:10" ht="45.75" hidden="1" thickBot="1">
       <c r="A85" s="5">
         <v>69</v>
       </c>
@@ -7853,7 +8309,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="33.75">
+    <row r="86" spans="1:10" ht="34.5" hidden="1" thickBot="1">
       <c r="A86" s="5">
         <v>70</v>
       </c>
@@ -7886,7 +8342,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="45">
+    <row r="87" spans="1:10" ht="45.75" hidden="1" thickBot="1">
       <c r="A87" s="5">
         <v>71</v>
       </c>
@@ -7917,7 +8373,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="22.5">
+    <row r="88" spans="1:10" ht="23.25" hidden="1" thickBot="1">
       <c r="A88" s="5">
         <v>72</v>
       </c>
@@ -7948,7 +8404,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="45">
+    <row r="89" spans="1:10" ht="45.75" hidden="1" thickBot="1">
       <c r="A89" s="5">
         <v>73</v>
       </c>
@@ -7979,7 +8435,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="25.5">
+    <row r="90" spans="1:10" ht="26.25" hidden="1" thickBot="1">
       <c r="A90" s="5">
         <v>74</v>
       </c>
@@ -8010,7 +8466,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="36" customHeight="1">
+    <row r="91" spans="1:10" ht="36" hidden="1" customHeight="1">
       <c r="A91" s="5">
         <v>75</v>
       </c>
@@ -8041,7 +8497,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="67.5">
+    <row r="92" spans="1:10" ht="68.25" hidden="1" thickBot="1">
       <c r="A92" s="5">
         <v>76</v>
       </c>
@@ -8072,7 +8528,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="33.75">
+    <row r="93" spans="1:10" ht="34.5" hidden="1" thickBot="1">
       <c r="A93" s="5">
         <v>77</v>
       </c>
@@ -8103,7 +8559,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="67.5">
+    <row r="94" spans="1:10" ht="68.25" hidden="1" thickBot="1">
       <c r="A94" s="5">
         <v>78</v>
       </c>
@@ -8136,7 +8592,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="45">
+    <row r="95" spans="1:10" ht="45.75" hidden="1" thickBot="1">
       <c r="A95" s="5">
         <v>79</v>
       </c>
@@ -8169,7 +8625,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="15" thickBot="1">
+    <row r="96" spans="1:10" ht="15" hidden="1" thickBot="1">
       <c r="A96" s="5">
         <v>80</v>
       </c>
@@ -8338,7 +8794,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="57" thickBot="1">
+    <row r="101" spans="1:12" ht="57" hidden="1" thickBot="1">
       <c r="A101" s="5">
         <v>85</v>
       </c>
@@ -8403,7 +8859,7 @@
       </c>
       <c r="J102" s="37"/>
     </row>
-    <row r="103" spans="1:12" ht="34.5" thickBot="1">
+    <row r="103" spans="1:12" ht="34.5" hidden="1" thickBot="1">
       <c r="A103" s="5">
         <v>87</v>
       </c>
@@ -8432,7 +8888,7 @@
       </c>
       <c r="J103" s="37"/>
     </row>
-    <row r="104" spans="1:12" ht="45.75" thickBot="1">
+    <row r="104" spans="1:12" ht="45.75" hidden="1" thickBot="1">
       <c r="A104" s="5">
         <v>88</v>
       </c>
@@ -8463,7 +8919,7 @@
       </c>
       <c r="J104" s="37"/>
     </row>
-    <row r="105" spans="1:12" ht="57" thickBot="1">
+    <row r="105" spans="1:12" ht="57" hidden="1" thickBot="1">
       <c r="A105" s="5">
         <v>89</v>
       </c>
@@ -8494,7 +8950,7 @@
       </c>
       <c r="J105" s="37"/>
     </row>
-    <row r="106" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
+    <row r="106" spans="1:12" ht="16.5" hidden="1" customHeight="1" thickBot="1">
       <c r="A106" s="5">
         <v>90</v>
       </c>
@@ -8523,7 +8979,7 @@
       </c>
       <c r="J106" s="37"/>
     </row>
-    <row r="107" spans="1:12" ht="45.75" thickBot="1">
+    <row r="107" spans="1:12" ht="45.75" hidden="1" thickBot="1">
       <c r="A107" s="5">
         <v>91</v>
       </c>
@@ -8591,7 +9047,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="79.5" thickBot="1">
+    <row r="109" spans="1:12" ht="78.75" hidden="1">
       <c r="A109" s="5">
         <v>93</v>
       </c>
@@ -8622,7 +9078,7 @@
       </c>
       <c r="J109" s="37"/>
     </row>
-    <row r="110" spans="1:12" ht="45.75" thickBot="1">
+    <row r="110" spans="1:12" ht="45.75" hidden="1" thickBot="1">
       <c r="A110" s="5"/>
       <c r="B110" s="57" t="s">
         <v>32</v>
@@ -8649,7 +9105,7 @@
       </c>
       <c r="J110" s="37"/>
     </row>
-    <row r="111" spans="1:12" ht="45.75" thickBot="1">
+    <row r="111" spans="1:12" ht="45.75" hidden="1" thickBot="1">
       <c r="A111" s="5"/>
       <c r="B111" s="58" t="s">
         <v>60</v>
@@ -8678,7 +9134,7 @@
       </c>
       <c r="J111" s="37"/>
     </row>
-    <row r="112" spans="1:12" ht="45">
+    <row r="112" spans="1:12" ht="45" hidden="1">
       <c r="A112" s="5"/>
       <c r="B112" s="24" t="s">
         <v>61</v>
@@ -8705,7 +9161,7 @@
       </c>
       <c r="J112" s="37"/>
     </row>
-    <row r="113" spans="1:12" ht="45">
+    <row r="113" spans="1:12" ht="45" hidden="1">
       <c r="A113" s="5"/>
       <c r="B113" s="24" t="s">
         <v>62</v>
@@ -8734,7 +9190,7 @@
       </c>
       <c r="J113" s="37"/>
     </row>
-    <row r="114" spans="1:12" ht="33.75">
+    <row r="114" spans="1:12" ht="33.75" hidden="1">
       <c r="A114" s="5"/>
       <c r="B114" s="24" t="s">
         <v>63</v>
@@ -8761,7 +9217,7 @@
       </c>
       <c r="J114" s="37"/>
     </row>
-    <row r="115" spans="1:12" ht="42.75" customHeight="1">
+    <row r="115" spans="1:12" ht="42.75" hidden="1" customHeight="1">
       <c r="A115" s="5"/>
       <c r="B115" s="25" t="s">
         <v>64</v>
@@ -8790,7 +9246,7 @@
       </c>
       <c r="J115" s="37"/>
     </row>
-    <row r="116" spans="1:12" ht="33.75">
+    <row r="116" spans="1:12" ht="33.75" hidden="1">
       <c r="A116" s="5"/>
       <c r="B116" s="23" t="s">
         <v>33</v>
@@ -8819,7 +9275,7 @@
       </c>
       <c r="J116" s="37"/>
     </row>
-    <row r="117" spans="1:12" ht="33.75">
+    <row r="117" spans="1:12" ht="33.75" hidden="1">
       <c r="A117" s="28"/>
       <c r="B117" s="24" t="s">
         <v>65</v>
@@ -8858,19 +9314,19 @@
       <c r="E118" s="45"/>
       <c r="F118" s="46">
         <f>SUBTOTAL(103,[Strefa])</f>
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="G118" s="46">
         <f>SUBTOTAL(109,[Liczba (sztuki)])</f>
-        <v>822</v>
+        <v>216</v>
       </c>
       <c r="H118" s="47">
         <f>SUBTOTAL(101,[Średnia cena])</f>
-        <v>33.540259740259742</v>
+        <v>42.547619047619051</v>
       </c>
       <c r="I118" s="46">
         <f>SUBTOTAL(109,[Suma])</f>
-        <v>9395.5</v>
+        <v>6102.5</v>
       </c>
       <c r="J118" s="46"/>
       <c r="K118" s="48"/>
@@ -9139,10 +9595,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9294,6 +9750,9 @@
       <c r="F10" s="67"/>
       <c r="G10" s="68"/>
       <c r="H10" s="68"/>
+      <c r="I10" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="33" customHeight="1">
       <c r="A11" s="65"/>
@@ -9439,7 +9898,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="33" customHeight="1">
+    <row r="17" spans="1:10" ht="33" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
@@ -9463,7 +9922,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="33" customHeight="1">
+    <row r="18" spans="1:10" ht="33" customHeight="1">
       <c r="A18" s="65">
         <v>15</v>
       </c>
@@ -9490,8 +9949,11 @@
       <c r="H18" s="70" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="33" customHeight="1">
+      <c r="I18" s="81">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="33" customHeight="1">
       <c r="A19" s="65"/>
       <c r="B19" s="63"/>
       <c r="C19" s="61"/>
@@ -9512,7 +9974,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="33" customHeight="1">
+    <row r="20" spans="1:10" ht="33" customHeight="1">
       <c r="A20" s="65"/>
       <c r="B20" s="63"/>
       <c r="C20" s="61"/>
@@ -9533,7 +9995,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="33" customHeight="1">
+    <row r="21" spans="1:10" ht="33" customHeight="1">
       <c r="A21" s="65"/>
       <c r="B21" s="63"/>
       <c r="C21" s="61"/>
@@ -9555,7 +10017,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="33" customHeight="1">
+    <row r="22" spans="1:10" ht="33" customHeight="1">
       <c r="A22" s="65"/>
       <c r="B22" s="63"/>
       <c r="C22" s="61"/>
@@ -9579,7 +10041,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="33" customHeight="1">
+    <row r="23" spans="1:10" ht="33" customHeight="1">
       <c r="A23" s="65"/>
       <c r="B23" s="63"/>
       <c r="C23" s="61"/>
@@ -9600,7 +10062,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="33" customHeight="1">
+    <row r="24" spans="1:10" ht="33" customHeight="1">
       <c r="A24" s="65"/>
       <c r="B24" s="63"/>
       <c r="C24" s="61"/>
@@ -9621,7 +10083,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="33" customHeight="1">
+    <row r="25" spans="1:10" ht="33" customHeight="1">
       <c r="A25" s="65"/>
       <c r="B25" s="63"/>
       <c r="C25" s="61"/>
@@ -9645,7 +10107,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="33" customHeight="1">
+    <row r="26" spans="1:10" ht="33" customHeight="1">
       <c r="A26" s="65">
         <v>16</v>
       </c>
@@ -9675,7 +10137,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="40.5" customHeight="1">
+    <row r="27" spans="1:10" ht="40.5" customHeight="1">
       <c r="A27" s="65">
         <v>30</v>
       </c>
@@ -9701,8 +10163,11 @@
       <c r="H27" s="70" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="40.5" customHeight="1">
+      <c r="J27" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="40.5" customHeight="1">
       <c r="A28" s="65"/>
       <c r="B28" s="63"/>
       <c r="C28" s="61"/>
@@ -9723,7 +10188,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="40.5" customHeight="1">
+    <row r="29" spans="1:10" ht="40.5" customHeight="1">
       <c r="A29" s="65"/>
       <c r="B29" s="63"/>
       <c r="C29" s="61"/>
@@ -9744,7 +10209,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="40.5" customHeight="1">
+    <row r="30" spans="1:10" ht="40.5" customHeight="1">
       <c r="A30" s="65"/>
       <c r="B30" s="63"/>
       <c r="C30" s="61"/>
@@ -9765,7 +10230,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="40.5" customHeight="1">
+    <row r="31" spans="1:10" ht="40.5" customHeight="1">
       <c r="A31" s="65"/>
       <c r="B31" s="63"/>
       <c r="C31" s="61"/>
@@ -9789,7 +10254,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="33" customHeight="1">
+    <row r="32" spans="1:10" ht="33" customHeight="1">
       <c r="A32" s="65">
         <v>35</v>
       </c>
@@ -10066,9 +10531,36 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="33" customHeight="1"/>
-    <row r="45" spans="1:9" ht="33" customHeight="1"/>
-    <row r="46" spans="1:9" ht="33" customHeight="1"/>
-    <row r="47" spans="1:9" ht="33" customHeight="1"/>
+    <row r="45" spans="1:9" ht="33" customHeight="1">
+      <c r="C45" t="s">
+        <v>429</v>
+      </c>
+      <c r="D45" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="33" customHeight="1">
+      <c r="B46" t="s">
+        <v>427</v>
+      </c>
+      <c r="C46" t="s">
+        <v>431</v>
+      </c>
+      <c r="D46" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="33" customHeight="1">
+      <c r="B47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C47" t="s">
+        <v>431</v>
+      </c>
+      <c r="D47" t="s">
+        <v>431</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10076,193 +10568,543 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="N5:P21"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="7" max="7" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.125" customWidth="1"/>
+    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="14:16">
-      <c r="N5">
-        <v>5.2</v>
-      </c>
-      <c r="O5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="P5">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="6" spans="14:16">
-      <c r="N6">
-        <v>2.5</v>
-      </c>
-      <c r="O6">
-        <v>1.7</v>
-      </c>
-      <c r="P6">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="7" spans="14:16">
-      <c r="N7">
-        <v>0.6</v>
-      </c>
-      <c r="O7">
-        <v>1.5</v>
-      </c>
-      <c r="P7">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="8" spans="14:16">
-      <c r="N8">
-        <v>1.3</v>
-      </c>
-      <c r="O8">
-        <v>1.5</v>
-      </c>
-      <c r="P8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="14:16">
-      <c r="N9">
-        <v>1.6</v>
-      </c>
-      <c r="O9">
-        <v>1.5</v>
-      </c>
-      <c r="P9">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="10" spans="14:16">
-      <c r="N10">
-        <v>1.3</v>
-      </c>
-      <c r="O10">
-        <v>1.5</v>
-      </c>
-      <c r="P10">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="11" spans="14:16">
-      <c r="N11">
-        <v>1.7</v>
-      </c>
-      <c r="O11">
-        <v>1.5</v>
-      </c>
-      <c r="P11">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="12" spans="14:16">
-      <c r="N12">
-        <v>1.5</v>
-      </c>
-      <c r="O12">
-        <v>1.5</v>
-      </c>
-      <c r="P12">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="13" spans="14:16">
-      <c r="N13">
-        <v>1.6</v>
-      </c>
-      <c r="O13">
-        <v>1.5</v>
-      </c>
-      <c r="P13">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="14" spans="14:16">
-      <c r="N14">
-        <v>1.9</v>
-      </c>
-      <c r="O14">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="P14">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="14:16">
-      <c r="N15">
-        <v>1.5</v>
-      </c>
-      <c r="O15">
-        <v>6.6</v>
-      </c>
-      <c r="P15">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="16" spans="14:16">
-      <c r="N16">
-        <v>1.6</v>
-      </c>
-      <c r="O16">
-        <v>4.5</v>
-      </c>
-      <c r="P16">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="17" spans="14:16">
-      <c r="N17">
-        <v>1.6</v>
-      </c>
-      <c r="O17">
-        <v>1.2</v>
-      </c>
-      <c r="P17">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="18" spans="14:16">
-      <c r="N18">
-        <v>8.5</v>
-      </c>
-      <c r="O18">
-        <v>5.8</v>
-      </c>
-      <c r="P18">
-        <v>6.05</v>
-      </c>
-    </row>
-    <row r="19" spans="14:16">
-      <c r="N19">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="20" spans="14:16">
-      <c r="N20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="14:16">
-      <c r="N21">
-        <f>SUM(N5:N20)</f>
-        <v>40.800000000000004</v>
-      </c>
-      <c r="O21">
-        <f>SUM(O5:O20)</f>
-        <v>40.699999999999996</v>
-      </c>
-      <c r="P21">
-        <f>SUM(P5:P20)</f>
-        <v>40.549999999999997</v>
+    <row r="1" spans="1:12" ht="15">
+      <c r="A1" s="82" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" s="84" t="s">
+        <v>371</v>
+      </c>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="L1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="E2" s="88" t="s">
+        <v>370</v>
+      </c>
+      <c r="F2" s="89" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" s="89" t="s">
+        <v>373</v>
+      </c>
+      <c r="H2" s="89" t="s">
+        <v>374</v>
+      </c>
+      <c r="K2" s="66" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="57">
+      <c r="A3" s="83" t="s">
+        <v>327</v>
+      </c>
+      <c r="E3" s="73" t="s">
+        <v>375</v>
+      </c>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85" t="s">
+        <v>377</v>
+      </c>
+      <c r="H3" s="85" t="s">
+        <v>376</v>
+      </c>
+      <c r="K3" s="66" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60">
+      <c r="E4" s="92" t="s">
+        <v>378</v>
+      </c>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93" t="s">
+        <v>379</v>
+      </c>
+      <c r="H4" s="93" t="s">
+        <v>380</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="71.25">
+      <c r="E5" s="73" t="s">
+        <v>383</v>
+      </c>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85" t="s">
+        <v>382</v>
+      </c>
+      <c r="H5" s="85" t="s">
+        <v>381</v>
+      </c>
+      <c r="I5" s="66"/>
+    </row>
+    <row r="6" spans="1:12" ht="42.75">
+      <c r="E6" s="86" t="s">
+        <v>384</v>
+      </c>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87" t="s">
+        <v>386</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>385</v>
+      </c>
+      <c r="I6" s="87" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="42.75">
+      <c r="A7" s="83" t="s">
+        <v>328</v>
+      </c>
+      <c r="E7" s="96" t="s">
+        <v>391</v>
+      </c>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97" t="s">
+        <v>393</v>
+      </c>
+      <c r="H7" s="97" t="s">
+        <v>392</v>
+      </c>
+      <c r="I7" s="66"/>
+    </row>
+    <row r="8" spans="1:12" ht="28.5">
+      <c r="E8" s="73" t="s">
+        <v>394</v>
+      </c>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85" t="s">
+        <v>395</v>
+      </c>
+      <c r="I8" s="66"/>
+    </row>
+    <row r="9" spans="1:12" ht="15">
+      <c r="E9" s="90" t="s">
+        <v>396</v>
+      </c>
+      <c r="F9" s="90"/>
+      <c r="G9" s="91" t="s">
+        <v>398</v>
+      </c>
+      <c r="H9" s="90" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15">
+      <c r="E10" s="94" t="s">
+        <v>399</v>
+      </c>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94" t="s">
+        <v>401</v>
+      </c>
+      <c r="H10" s="94" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15">
+      <c r="A11" s="83" t="s">
+        <v>329</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>402</v>
+      </c>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88" t="s">
+        <v>404</v>
+      </c>
+      <c r="H11" s="88" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15">
+      <c r="E12" s="88" t="s">
+        <v>344</v>
+      </c>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88" t="s">
+        <v>406</v>
+      </c>
+      <c r="H12" s="88" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15">
+      <c r="E13" s="90" t="s">
+        <v>407</v>
+      </c>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90" t="s">
+        <v>409</v>
+      </c>
+      <c r="H13" s="90" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="E14" s="73" t="s">
+        <v>410</v>
+      </c>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73" t="s">
+        <v>412</v>
+      </c>
+      <c r="H14" s="73" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="83" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>354</v>
+      </c>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73" t="s">
+        <v>414</v>
+      </c>
+      <c r="H15" s="73" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15">
+      <c r="E16" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="E17" s="73" t="s">
+        <v>417</v>
+      </c>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73" t="s">
+        <v>418</v>
+      </c>
+      <c r="H17" s="73" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15">
+      <c r="E18" s="90" t="s">
+        <v>362</v>
+      </c>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90" t="s">
+        <v>421</v>
+      </c>
+      <c r="H18" s="90" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="83" t="s">
+        <v>331</v>
+      </c>
+      <c r="E19" s="73" t="s">
+        <v>422</v>
+      </c>
+      <c r="G19" s="73" t="s">
+        <v>423</v>
+      </c>
+      <c r="H19">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15">
+      <c r="E20" s="92" t="s">
+        <v>424</v>
+      </c>
+      <c r="F20" s="95"/>
+      <c r="G20" s="92" t="s">
+        <v>426</v>
+      </c>
+      <c r="H20" s="95" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15">
+      <c r="A23" s="82" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="83" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="83" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="83" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="83" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15">
+      <c r="A43" s="82" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="83" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="83" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="83" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="83" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="83" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="83" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="83" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="83" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="83" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="83" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="83" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="83" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="83" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="83" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="83" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A11" r:id="rId3"/>
+    <hyperlink ref="A15" r:id="rId4"/>
+    <hyperlink ref="A19" r:id="rId5"/>
+    <hyperlink ref="A27" r:id="rId6"/>
+    <hyperlink ref="A33" r:id="rId7"/>
+    <hyperlink ref="A37" r:id="rId8" display="http://zielony-zywoplot.pl/"/>
+    <hyperlink ref="A39" r:id="rId9"/>
+    <hyperlink ref="A47" r:id="rId10"/>
+    <hyperlink ref="A53" r:id="rId11"/>
+    <hyperlink ref="A59" r:id="rId12"/>
+    <hyperlink ref="A63" r:id="rId13" display="http://allegro.pl/rosliny-drzewa-i-krzewy-iglaste-99745"/>
+    <hyperlink ref="A75" r:id="rId14" display="http://allegro.pl/rosliny-trawy-99817"/>
+    <hyperlink ref="A79" r:id="rId15"/>
+    <hyperlink ref="A85" r:id="rId16"/>
+    <hyperlink ref="A91" r:id="rId17"/>
+    <hyperlink ref="A95" r:id="rId18" display="http://allegro.pl/rosliny-drzewa-i-krzewy-lisciaste-99754"/>
+    <hyperlink ref="A107" r:id="rId19"/>
+    <hyperlink ref="A113" r:id="rId20"/>
+    <hyperlink ref="A119" r:id="rId21"/>
+    <hyperlink ref="A125" r:id="rId22"/>
+    <hyperlink ref="A131" r:id="rId23"/>
+    <hyperlink ref="A135" r:id="rId24" display="http://allegro.pl/rosliny-byliny-ozdobne-99806"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>